<commit_message>
Chapters 13 and 14 completed
Chapters 13 (HIV Knowledge, Attitudes and Behaviors) and 14 (HIV Prevalence) are completed.

Update of Indicator list and Readme files
</commit_message>
<xml_diff>
--- a/DHS7tabplan/Tab_plan_Chap16_Adult_Maternal_Mortality.xlsx
+++ b/DHS7tabplan/Tab_plan_Chap16_Adult_Maternal_Mortality.xlsx
@@ -4657,8 +4657,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="480" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4112082b3fcc37184355d8d9f746cc16">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e31d9155d0f1567779179698607192e" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="481" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be21cae339529f0f311ef097f4a87693">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd9e5a0c56088652e9b5d1a36fcd7f8a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <xsd:import namespace="d16efad5-0601-4cf0-b7c2-89968258c777"/>
@@ -4955,7 +4955,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C0105CD-E45A-43DA-8E37-06B050401342}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D930BF3-A295-45F6-BB59-E1DB12A9DCE3}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>